<commit_message>
Show UI when List and Regex rules fail
</commit_message>
<xml_diff>
--- a/DataValidationRules.xlsx
+++ b/DataValidationRules.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t xml:space="preserve">Category</t>
   </si>
@@ -40,27 +40,6 @@
     <t xml:space="preserve">User Visible Message</t>
   </si>
   <si>
-    <t xml:space="preserve">Doors</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fire Rating</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FromHostType</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;Function&gt;-&lt;Fire Rating&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">In Room Bounding Wall</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FromHostInstance</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;Room Bounding&gt;</t>
-  </si>
-  <si>
     <t xml:space="preserve">Floors</t>
   </si>
   <si>
@@ -70,37 +49,31 @@
     <t xml:space="preserve">List</t>
   </si>
   <si>
-    <t xml:space="preserve">1,2,3</t>
+    <t xml:space="preserve">the,quick,brown,fox</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Y</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enter a value from “the quick brown fox”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;all&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mark</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Regex</t>
+  </si>
+  <si>
+    <t xml:space="preserve">^\d+$</t>
   </si>
   <si>
     <t xml:space="preserve">N</t>
   </si>
   <si>
-    <t xml:space="preserve">Allowable values for floor comments are 1,2,3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Zipcode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Regex</t>
-  </si>
-  <si>
-    <t xml:space="preserve">^\d{5}(-?\d{4})?$</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Y</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Enter a 5 or 9 digit zip code such as 02134 or 02134-1433</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Info</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PreventDuplicates</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Duplicate values are not allowed for the Floor Info parameter</t>
+    <t xml:space="preserve">Mark must contain only numbers</t>
   </si>
 </sst>
 </file>
@@ -182,7 +155,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -193,6 +166,14 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
@@ -216,10 +197,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F1006"/>
+  <dimension ref="A1:F1002"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
+      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -266,74 +247,38 @@
       <c r="D2" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="E2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="3" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
-    <row r="4" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
+    <row r="4" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="5" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="6" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>26</v>
-      </c>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
     </row>
     <row r="7" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="8" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1331,10 +1276,6 @@
     <row r="1000" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1001" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1002" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1003" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1004" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1005" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1006" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>